<commit_message>
making multiple parameters checks
</commit_message>
<xml_diff>
--- a/Results/apriori_top_category_combinations.xlsx
+++ b/Results/apriori_top_category_combinations.xlsx
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11">

</xml_diff>